<commit_message>
Luận xong Tật Ách
</commit_message>
<xml_diff>
--- a/LuanTatAch.xlsx
+++ b/LuanTatAch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CBC9F7-2548-45DF-9011-B3E74D8657CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4502A14-AC6F-41FB-AB45-EF4DC073FBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7622" uniqueCount="3734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7698" uniqueCount="3772">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -11227,6 +11227,120 @@
   </si>
   <si>
     <t>Thai Phụ tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Hóa Quyền, Lộc Tồn đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Hóa Lộc, Lộc Tồn, Bác Sỹ đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Hóa Kỵ đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Hóa Kỵ đồng cung tại Tật Ách ở Dần</t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Hóa Kỵ đồng cung tại Tật Ách ở Thân</t>
+  </si>
+  <si>
+    <t>Hóa Kỵ, Thiên Đồng đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Vũ Khúc, Tham Lang, Văn Xương, Văn Khúc đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Vũ Khúc, Thiên Riêu đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Vũ Khúc, Thiên Riêu, Phá Toái, Thiên Việt đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thái Dương, Thiên Riêu, Đà La, Hóa Kỵ đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thái Dương, Thiên Hình đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thái Dương, Long Trì đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thiên Cơ, Thiên Hình, Địa Không, Địa Kiếp đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thiên Cơ, Kình Dương, Đà La đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thiên Cơ, Thiên Khốc, Thiên Hư đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thái Âm, Thiên Riêu, Đà La, Hóa Kỵ đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thái Âm Thiên Hình đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Tham Lang, Thiên Riêu đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Tham Lang, Hóa Kỵ đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Cự Môn, Kình Dương, Hỏa Tinh đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Cự Môn, Hóa Kỵ đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thiên Tướng, Thiên Hình đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thất Sát, Đại Hao, Tiểu Hao, Hóa Kỵ đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thất Sát, Thiên Hình, Đà La, Phá Quân đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Phá Quân, Thiên Hình, Phục Binh, Địa Không đồng cung tại Tật Ách"</t>
+  </si>
+  <si>
+    <t>Phá Quân, Thiên Hình, Hóa Kỵ, Kình Dương đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>ình Dương, Hỏa Tinh, Linh Tinh, Địa Không, Địa Kiếp đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Kình Dương, Thiên Hình, Địa Không, Địa Kiếp đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Kình Dương, Thiên Hình đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Kình Dương, Hỏa Tinh, Linh Tinh, Lưu Hà đồng cung tại Tật Ách ở Thìn</t>
+  </si>
+  <si>
+    <t>Tang Môn, Điếu Khách, Hóa Kỵ đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thiên Mã, Thiên Hình đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thái Tuế, Thiên Hình, Thiên Mã, Kiếp Sát đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Tang Môn, Điếu Khách đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thiên Khốc, Thiên Hư, Tang Môn, Bạch Hổ đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thiên Riêu, Thiên Hình, Địa Không, Địa Kiếp đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Đào Hoa, Hồng Loan, Địa Không, Địa Kiếp đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Đào Hoa, Hồng Loan, Kình Dương, Hóa Kỵ đồng cung tại Tật Ách</t>
   </si>
 </sst>
 </file>
@@ -11765,10 +11879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B3812"/>
+  <dimension ref="A1:B3851"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1652" workbookViewId="0">
-      <selection activeCell="R1660" sqref="R1660"/>
+    <sheetView tabSelected="1" topLeftCell="A3821" workbookViewId="0">
+      <selection activeCell="B3851" sqref="B3851"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42262,6 +42376,310 @@
       </c>
       <c r="B3812" t="s">
         <v>3612</v>
+      </c>
+    </row>
+    <row r="3814" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3814" t="s">
+        <v>3734</v>
+      </c>
+      <c r="B3814" t="s">
+        <v>3734</v>
+      </c>
+    </row>
+    <row r="3815" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3815" t="s">
+        <v>3735</v>
+      </c>
+      <c r="B3815" t="s">
+        <v>3735</v>
+      </c>
+    </row>
+    <row r="3816" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3816" t="s">
+        <v>3736</v>
+      </c>
+      <c r="B3816" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="3817" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3817" t="s">
+        <v>3737</v>
+      </c>
+      <c r="B3817" t="s">
+        <v>3737</v>
+      </c>
+    </row>
+    <row r="3818" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3818" t="s">
+        <v>3738</v>
+      </c>
+      <c r="B3818" t="s">
+        <v>3738</v>
+      </c>
+    </row>
+    <row r="3819" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3819" t="s">
+        <v>3739</v>
+      </c>
+      <c r="B3819" t="s">
+        <v>3739</v>
+      </c>
+    </row>
+    <row r="3820" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3820" t="s">
+        <v>3740</v>
+      </c>
+      <c r="B3820" t="s">
+        <v>3740</v>
+      </c>
+    </row>
+    <row r="3821" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3821" t="s">
+        <v>3741</v>
+      </c>
+      <c r="B3821" t="s">
+        <v>3741</v>
+      </c>
+    </row>
+    <row r="3822" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3822" t="s">
+        <v>3742</v>
+      </c>
+      <c r="B3822" t="s">
+        <v>3742</v>
+      </c>
+    </row>
+    <row r="3823" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3823" t="s">
+        <v>3743</v>
+      </c>
+      <c r="B3823" t="s">
+        <v>3743</v>
+      </c>
+    </row>
+    <row r="3824" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3824" t="s">
+        <v>3744</v>
+      </c>
+      <c r="B3824" t="s">
+        <v>3744</v>
+      </c>
+    </row>
+    <row r="3825" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3825" t="s">
+        <v>3745</v>
+      </c>
+      <c r="B3825" t="s">
+        <v>3745</v>
+      </c>
+    </row>
+    <row r="3826" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3826" t="s">
+        <v>3746</v>
+      </c>
+      <c r="B3826" t="s">
+        <v>3746</v>
+      </c>
+    </row>
+    <row r="3827" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3827" t="s">
+        <v>3747</v>
+      </c>
+      <c r="B3827" t="s">
+        <v>3747</v>
+      </c>
+    </row>
+    <row r="3828" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3828" t="s">
+        <v>3748</v>
+      </c>
+      <c r="B3828" t="s">
+        <v>3748</v>
+      </c>
+    </row>
+    <row r="3829" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3829" t="s">
+        <v>3749</v>
+      </c>
+      <c r="B3829" t="s">
+        <v>3749</v>
+      </c>
+    </row>
+    <row r="3830" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3830" t="s">
+        <v>3750</v>
+      </c>
+      <c r="B3830" t="s">
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="3831" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3831" t="s">
+        <v>3751</v>
+      </c>
+      <c r="B3831" t="s">
+        <v>3751</v>
+      </c>
+    </row>
+    <row r="3832" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3832" t="s">
+        <v>3752</v>
+      </c>
+      <c r="B3832" t="s">
+        <v>3752</v>
+      </c>
+    </row>
+    <row r="3833" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3833" t="s">
+        <v>3753</v>
+      </c>
+      <c r="B3833" t="s">
+        <v>3753</v>
+      </c>
+    </row>
+    <row r="3834" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3834" t="s">
+        <v>3754</v>
+      </c>
+      <c r="B3834" t="s">
+        <v>3754</v>
+      </c>
+    </row>
+    <row r="3835" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3835" t="s">
+        <v>3755</v>
+      </c>
+      <c r="B3835" t="s">
+        <v>3755</v>
+      </c>
+    </row>
+    <row r="3836" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3836" t="s">
+        <v>3756</v>
+      </c>
+      <c r="B3836" t="s">
+        <v>3756</v>
+      </c>
+    </row>
+    <row r="3837" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3837" t="s">
+        <v>3757</v>
+      </c>
+      <c r="B3837" t="s">
+        <v>3757</v>
+      </c>
+    </row>
+    <row r="3838" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3838" t="s">
+        <v>3758</v>
+      </c>
+      <c r="B3838" t="s">
+        <v>3758</v>
+      </c>
+    </row>
+    <row r="3839" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3839" t="s">
+        <v>3759</v>
+      </c>
+      <c r="B3839" t="s">
+        <v>3759</v>
+      </c>
+    </row>
+    <row r="3840" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3840" t="s">
+        <v>3760</v>
+      </c>
+      <c r="B3840" t="s">
+        <v>3760</v>
+      </c>
+    </row>
+    <row r="3841" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3841" t="s">
+        <v>3761</v>
+      </c>
+      <c r="B3841" t="s">
+        <v>3761</v>
+      </c>
+    </row>
+    <row r="3842" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3842" t="s">
+        <v>3762</v>
+      </c>
+      <c r="B3842" t="s">
+        <v>3762</v>
+      </c>
+    </row>
+    <row r="3843" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3843" t="s">
+        <v>3763</v>
+      </c>
+      <c r="B3843" t="s">
+        <v>3763</v>
+      </c>
+    </row>
+    <row r="3844" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3844" t="s">
+        <v>3764</v>
+      </c>
+      <c r="B3844" t="s">
+        <v>3764</v>
+      </c>
+    </row>
+    <row r="3845" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3845" t="s">
+        <v>3765</v>
+      </c>
+      <c r="B3845" t="s">
+        <v>3765</v>
+      </c>
+    </row>
+    <row r="3846" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3846" t="s">
+        <v>3766</v>
+      </c>
+      <c r="B3846" t="s">
+        <v>3766</v>
+      </c>
+    </row>
+    <row r="3847" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3847" t="s">
+        <v>3767</v>
+      </c>
+      <c r="B3847" t="s">
+        <v>3767</v>
+      </c>
+    </row>
+    <row r="3848" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3848" t="s">
+        <v>3768</v>
+      </c>
+      <c r="B3848" t="s">
+        <v>3768</v>
+      </c>
+    </row>
+    <row r="3849" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3849" t="s">
+        <v>3769</v>
+      </c>
+      <c r="B3849" t="s">
+        <v>3769</v>
+      </c>
+    </row>
+    <row r="3850" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3850" t="s">
+        <v>3770</v>
+      </c>
+      <c r="B3850" t="s">
+        <v>3770</v>
+      </c>
+    </row>
+    <row r="3851" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3851" t="s">
+        <v>3771</v>
+      </c>
+      <c r="B3851" t="s">
+        <v>3771</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Giải thích xong Tham Lang
</commit_message>
<xml_diff>
--- a/LuanTatAch.xlsx
+++ b/LuanTatAch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853F7D6D-3CBF-4DB8-A86B-386CC001A130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECF08E6-8518-44E5-B792-882F317EB044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8952" uniqueCount="4487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9020" uniqueCount="4560">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13489,6 +13489,227 @@
   </si>
   <si>
     <t>Bệnh tình, tai ương phải mổ sẻ, phẫu thuật</t>
+  </si>
+  <si>
+    <t>Có tỳ vết ở chân tay hay ở lưng</t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Tham Lang đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Mắt kém, hay mắc tù tội.</t>
+  </si>
+  <si>
+    <t>Dễ tự tử</t>
+  </si>
+  <si>
+    <t>Tham Lang, Liêm Trinh, Hỏa Tinh đồng cung tại cung Tật Ách</t>
+  </si>
+  <si>
+    <t>Dễ tử tự</t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Tham Lang, Địa Không, Địa Kiếp đồng cung tại cung Tật Ách</t>
+  </si>
+  <si>
+    <t>Tai nạn khủng khiếp</t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Thất Sát đồng cung tại cung Tật Ách</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mắt rất kém, mắc tai nạn xe cộ hay đao thương. </t>
+  </si>
+  <si>
+    <t>Chết bất đắc kỳ tử, hoặc vì mắc tai nạn, hoặc  vì ngộ độc.</t>
+  </si>
+  <si>
+    <t>Đau bụng, bộ máy tiêu hóa không được lành mạnh.</t>
+  </si>
+  <si>
+    <t>Thiên Đồng, Cự Môn đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bệnh tâm khí </t>
+  </si>
+  <si>
+    <t>Thiên Đồng, Thái Âm đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Bệnh huyết khí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bệnh ngoài da, chân tay có tỳ vết. </t>
+  </si>
+  <si>
+    <t>Vũ Khúc, Thiên Tướng đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Có ám tật.</t>
+  </si>
+  <si>
+    <t>Tham Lang, Văn Xương, Văn Khúc đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhiều nốt ruồi, hay mắc bệnh có liên quan đến lông tóc. </t>
+  </si>
+  <si>
+    <t>Vũ Khúc, Thất Sát đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Bệnh ở bộ máy tiêu hóa.</t>
+  </si>
+  <si>
+    <t>yếu thận,  phù chân tay.</t>
+  </si>
+  <si>
+    <t>Riêu Việt Toái</t>
+  </si>
+  <si>
+    <t>Riêu Việt Toái hội chiếu tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Bệnh chậm nói, câm</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Tật Ách</t>
+  </si>
+  <si>
+    <t>Căng mạch máu, hay nhức đầu</t>
+  </si>
+  <si>
+    <t>Thái Dương, Thái Âm đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Bệnh nạn liên miên</t>
+  </si>
+  <si>
+    <t>Thái Dương sáng tại Tật Ách gặp Thiên Riêu, Hóa Kỵ, Đà La</t>
+  </si>
+  <si>
+    <t>Đau mắt,có tật ở mắt.</t>
+  </si>
+  <si>
+    <t>Thái Dương tối tại Tật Ách gặp Thiên Riêu, Hóa Kỵ, Đà La</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nếu không mù mắt, què chân cũng đau mắt nặng và 
+khản tiếng. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vật kim khí sắc nhọn đâm vào mắt. </t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Tật Ách</t>
+  </si>
+  <si>
+    <t>Thiên Cơ, Cự Môn đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bệnh khi huyết </t>
+  </si>
+  <si>
+    <t>Bệnh ngoài da hay bệnh tê thấp.</t>
+  </si>
+  <si>
+    <t>Thiên Cơ, Thiên Lương đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Bệnh ở hạ bộ.</t>
+  </si>
+  <si>
+    <t>Thiên Cơ, Thái Âm đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Có nhiều mụn nhọt</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Tật Ách gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Chân tay yếu gân.</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Tật Ách gặp Thiên Khốc, Thiên Hư</t>
+  </si>
+  <si>
+    <t>Bệnh phong đờm, ho ra máu</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Tật Ách gặp Thiên Hình, Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mắc bệnh tật hay tai nạn bất ngờ rất đáng lo ngại. </t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Tật Ách gặp Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Bệnh thần kinh</t>
+  </si>
+  <si>
+    <t>Hay đau bụng, hệ tiêu hóa kém</t>
+  </si>
+  <si>
+    <t>Thái Âm tối tại Tật Ách</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bệnh đau phổi </t>
+  </si>
+  <si>
+    <t>Thái Âm tối tại Tật Ách gặp Thiên Riêu, Hóa Kỵ, Đà La</t>
+  </si>
+  <si>
+    <t>Bị măt kém, mù lòa, dễ quáng gà</t>
+  </si>
+  <si>
+    <t>Thái Âm, Thiên Hình đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bị kim khí sắc nhọn đâm vào mắt. </t>
+  </si>
+  <si>
+    <t>Bệnh ở chân</t>
+  </si>
+  <si>
+    <t>Mắc tai nạn xe cộ hay bị súc vật cắn đá, nếu  không, cũng vì ăn uống mà sinh bệnh khó chữa.</t>
+  </si>
+  <si>
+    <t>Tham Lang, Đà La đồng cung tại Tật Ách ở Dần</t>
+  </si>
+  <si>
+    <t>Tham Lang, Đà La đồng cung tại Tật Ách ở Thân</t>
+  </si>
+  <si>
+    <t>Thú dữ cắn đá, nếu không, cũng mác tai nạn xe cộ 
+rất nguy hiểm.</t>
+  </si>
+  <si>
+    <t>Tham Lang, Bạch Hổ đồng cung tại Tật Ách ở Tuất</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dễ bị thú dữ cắn chết </t>
+  </si>
+  <si>
+    <t>Chơi bời, phóng túng, sinh hoạt không điều độ mà mắc bệnh.</t>
+  </si>
+  <si>
+    <t>Tham Lang, Hoá Kỵ đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Tai nạn sông nước</t>
+  </si>
+  <si>
+    <t>Tham Lang, Hoá Kỵ đồng cung tại Tật Ách gặp Thiên Lương</t>
+  </si>
+  <si>
+    <t>Dễ mắc kiện tụng, tù tội</t>
+  </si>
+  <si>
+    <t>Tham Lang, Hoá Kỵ, Thiên Riêu đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Tai nạn sông nước, hoặc bị bệnh phong tình</t>
   </si>
 </sst>
 </file>
@@ -14040,10 +14261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A2:B4477"/>
+  <dimension ref="A2:B4511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4231" workbookViewId="0">
-      <selection activeCell="F4251" sqref="F4251"/>
+    <sheetView tabSelected="1" topLeftCell="A4490" workbookViewId="0">
+      <selection activeCell="B4514" sqref="B4514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14792,7 +15013,7 @@
         <v>230</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>230</v>
+        <v>4487</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -17824,7 +18045,7 @@
         <v>604</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>604</v>
+        <v>4539</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
@@ -20432,7 +20653,7 @@
         <v>928</v>
       </c>
       <c r="B799" s="1" t="s">
-        <v>928</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.25">
@@ -23288,7 +23509,7 @@
         <v>1285</v>
       </c>
       <c r="B1156" s="1" t="s">
-        <v>1285</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="1157" spans="1:2" x14ac:dyDescent="0.25">
@@ -34571,12 +34792,12 @@
         <v>2443</v>
       </c>
     </row>
-    <row r="2567" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2567" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2567" s="1" t="s">
         <v>2444</v>
       </c>
       <c r="B2567" s="1" t="s">
-        <v>2444</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="2568" spans="1:2" x14ac:dyDescent="0.25">
@@ -34592,7 +34813,7 @@
         <v>2446</v>
       </c>
       <c r="B2569" s="1" t="s">
-        <v>2446</v>
+        <v>4546</v>
       </c>
     </row>
     <row r="2570" spans="1:2" x14ac:dyDescent="0.25">
@@ -34603,12 +34824,12 @@
         <v>2447</v>
       </c>
     </row>
-    <row r="2571" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2571" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2571" s="1" t="s">
         <v>2448</v>
       </c>
       <c r="B2571" s="1" t="s">
-        <v>2448</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="2572" spans="1:2" x14ac:dyDescent="0.25">
@@ -34619,12 +34840,12 @@
         <v>2449</v>
       </c>
     </row>
-    <row r="2573" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2573" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2573" s="1" t="s">
         <v>2450</v>
       </c>
       <c r="B2573" s="1" t="s">
-        <v>2450</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="2574" spans="1:2" x14ac:dyDescent="0.25">
@@ -34640,7 +34861,7 @@
         <v>2452</v>
       </c>
       <c r="B2575" s="1" t="s">
-        <v>2452</v>
+        <v>4546</v>
       </c>
     </row>
     <row r="2576" spans="1:2" x14ac:dyDescent="0.25">
@@ -34651,12 +34872,12 @@
         <v>2453</v>
       </c>
     </row>
-    <row r="2577" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2577" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2577" s="1" t="s">
         <v>2454</v>
       </c>
       <c r="B2577" s="1" t="s">
-        <v>2454</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="2578" spans="1:2" x14ac:dyDescent="0.25">
@@ -40616,7 +40837,7 @@
         <v>3199</v>
       </c>
       <c r="B3322" s="1" t="s">
-        <v>3199</v>
+        <v>4490</v>
       </c>
     </row>
     <row r="3323" spans="1:2" x14ac:dyDescent="0.25">
@@ -43947,20 +44168,20 @@
         <v>3736</v>
       </c>
     </row>
-    <row r="3739" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3739" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3739" s="1" t="s">
         <v>3737</v>
       </c>
       <c r="B3739" s="1" t="s">
-        <v>3737</v>
-      </c>
-    </row>
-    <row r="3740" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4497</v>
+      </c>
+    </row>
+    <row r="3740" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3740" s="1" t="s">
         <v>3738</v>
       </c>
       <c r="B3740" s="1" t="s">
-        <v>3738</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="3741" spans="1:2" x14ac:dyDescent="0.25">
@@ -49857,6 +50078,278 @@
       </c>
       <c r="B4477" s="1" t="s">
         <v>4479</v>
+      </c>
+    </row>
+    <row r="4478" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4478" s="1" t="s">
+        <v>4488</v>
+      </c>
+      <c r="B4478" s="1" t="s">
+        <v>4489</v>
+      </c>
+    </row>
+    <row r="4479" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4479" s="1" t="s">
+        <v>4491</v>
+      </c>
+      <c r="B4479" s="1" t="s">
+        <v>4492</v>
+      </c>
+    </row>
+    <row r="4480" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4480" s="1" t="s">
+        <v>4493</v>
+      </c>
+      <c r="B4480" s="1" t="s">
+        <v>4494</v>
+      </c>
+    </row>
+    <row r="4481" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4481" s="1" t="s">
+        <v>4495</v>
+      </c>
+      <c r="B4481" s="1" t="s">
+        <v>4496</v>
+      </c>
+    </row>
+    <row r="4482" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4482" s="1" t="s">
+        <v>4499</v>
+      </c>
+      <c r="B4482" s="1" t="s">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="4483" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4483" s="1" t="s">
+        <v>4501</v>
+      </c>
+      <c r="B4483" s="1" t="s">
+        <v>4502</v>
+      </c>
+    </row>
+    <row r="4484" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4484" s="1" t="s">
+        <v>4504</v>
+      </c>
+      <c r="B4484" s="1" t="s">
+        <v>4505</v>
+      </c>
+    </row>
+    <row r="4485" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4485" s="1" t="s">
+        <v>4506</v>
+      </c>
+      <c r="B4485" s="1" t="s">
+        <v>4507</v>
+      </c>
+    </row>
+    <row r="4486" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4486" s="1" t="s">
+        <v>4508</v>
+      </c>
+      <c r="B4486" s="1" t="s">
+        <v>4509</v>
+      </c>
+    </row>
+    <row r="4487" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4487" s="1" t="s">
+        <v>3741</v>
+      </c>
+      <c r="B4487" s="1" t="s">
+        <v>4510</v>
+      </c>
+    </row>
+    <row r="4488" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4488" s="1" t="s">
+        <v>4511</v>
+      </c>
+      <c r="B4488" s="1" t="s">
+        <v>4511</v>
+      </c>
+    </row>
+    <row r="4489" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4489" s="1" t="s">
+        <v>4512</v>
+      </c>
+      <c r="B4489" s="1" t="s">
+        <v>4513</v>
+      </c>
+    </row>
+    <row r="4490" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4490" s="1" t="s">
+        <v>4514</v>
+      </c>
+      <c r="B4490" s="1" t="s">
+        <v>4515</v>
+      </c>
+    </row>
+    <row r="4491" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4491" s="1" t="s">
+        <v>4516</v>
+      </c>
+      <c r="B4491" s="1" t="s">
+        <v>4517</v>
+      </c>
+    </row>
+    <row r="4492" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4492" s="1" t="s">
+        <v>4518</v>
+      </c>
+      <c r="B4492" s="1" t="s">
+        <v>4519</v>
+      </c>
+    </row>
+    <row r="4493" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4493" s="1" t="s">
+        <v>4520</v>
+      </c>
+      <c r="B4493" s="1" t="s">
+        <v>4521</v>
+      </c>
+    </row>
+    <row r="4494" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4494" s="1" t="s">
+        <v>3744</v>
+      </c>
+      <c r="B4494" s="1" t="s">
+        <v>4522</v>
+      </c>
+    </row>
+    <row r="4495" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4495" s="1" t="s">
+        <v>4523</v>
+      </c>
+      <c r="B4495" s="1" t="s">
+        <v>4526</v>
+      </c>
+    </row>
+    <row r="4496" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4496" s="1" t="s">
+        <v>4524</v>
+      </c>
+      <c r="B4496" s="1" t="s">
+        <v>4525</v>
+      </c>
+    </row>
+    <row r="4497" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4497" s="1" t="s">
+        <v>4527</v>
+      </c>
+      <c r="B4497" s="1" t="s">
+        <v>4528</v>
+      </c>
+    </row>
+    <row r="4498" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4498" s="1" t="s">
+        <v>4529</v>
+      </c>
+      <c r="B4498" s="1" t="s">
+        <v>4530</v>
+      </c>
+    </row>
+    <row r="4499" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4499" s="1" t="s">
+        <v>4531</v>
+      </c>
+      <c r="B4499" s="1" t="s">
+        <v>4532</v>
+      </c>
+    </row>
+    <row r="4500" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4500" s="1" t="s">
+        <v>4533</v>
+      </c>
+      <c r="B4500" s="1" t="s">
+        <v>4534</v>
+      </c>
+    </row>
+    <row r="4501" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4501" s="1" t="s">
+        <v>4535</v>
+      </c>
+      <c r="B4501" s="1" t="s">
+        <v>4536</v>
+      </c>
+    </row>
+    <row r="4502" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4502" s="1" t="s">
+        <v>4537</v>
+      </c>
+      <c r="B4502" s="1" t="s">
+        <v>4538</v>
+      </c>
+    </row>
+    <row r="4503" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4503" s="1" t="s">
+        <v>4540</v>
+      </c>
+      <c r="B4503" s="1" t="s">
+        <v>4541</v>
+      </c>
+    </row>
+    <row r="4504" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4504" s="1" t="s">
+        <v>4542</v>
+      </c>
+      <c r="B4504" s="1" t="s">
+        <v>4543</v>
+      </c>
+    </row>
+    <row r="4505" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4505" s="1" t="s">
+        <v>4544</v>
+      </c>
+      <c r="B4505" s="1" t="s">
+        <v>4545</v>
+      </c>
+    </row>
+    <row r="4506" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4506" s="1" t="s">
+        <v>4548</v>
+      </c>
+      <c r="B4506" s="1" t="s">
+        <v>4547</v>
+      </c>
+    </row>
+    <row r="4507" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4507" s="1" t="s">
+        <v>4549</v>
+      </c>
+      <c r="B4507" s="1" t="s">
+        <v>4547</v>
+      </c>
+    </row>
+    <row r="4508" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4508" s="1" t="s">
+        <v>4551</v>
+      </c>
+      <c r="B4508" s="1" t="s">
+        <v>4552</v>
+      </c>
+    </row>
+    <row r="4509" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4509" s="1" t="s">
+        <v>4554</v>
+      </c>
+      <c r="B4509" s="1" t="s">
+        <v>4555</v>
+      </c>
+    </row>
+    <row r="4510" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4510" s="1" t="s">
+        <v>4556</v>
+      </c>
+      <c r="B4510" s="1" t="s">
+        <v>4557</v>
+      </c>
+    </row>
+    <row r="4511" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4511" s="1" t="s">
+        <v>4558</v>
+      </c>
+      <c r="B4511" s="1" t="s">
+        <v>4559</v>
       </c>
     </row>
   </sheetData>
@@ -49877,43 +50370,43 @@
   <conditionalFormatting sqref="A146:A209">
     <cfRule type="duplicateValues" dxfId="16" priority="62"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6758:A1048576 A210:A1632 A2:A24 A26:A85 A144 A1805:A1809 A3442:A3852 A3915:A4214">
-    <cfRule type="duplicateValues" dxfId="15" priority="102"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="104"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A1810:A3339">
-    <cfRule type="duplicateValues" dxfId="13" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3853:A3914">
-    <cfRule type="duplicateValues" dxfId="12" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6758:A1048576 A210:A1632 A2:A24 A26:A85 A144 A1805:A1809 A3442:A3852 A3915:A4214">
+    <cfRule type="duplicateValues" dxfId="13" priority="102"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="104"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:B1048576">
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86:B143">
-    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B146:B209">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6758:B1048576 B210:B1632 B2:B24 B26:B85 B144 B1805:B1809 B3442:B3852 B3915:B4214">
-    <cfRule type="duplicateValues" dxfId="4" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1810:B3339">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3853:B3914">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="B6758:B1048576 B210:B1632 B2:B24 B26:B85 B144 B1805:B1809 B3915:B4214 B3442:B3852">
+    <cfRule type="duplicateValues" dxfId="1" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Giải thích Tật ách các chính tinh
</commit_message>
<xml_diff>
--- a/LuanTatAch.xlsx
+++ b/LuanTatAch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECF08E6-8518-44E5-B792-882F317EB044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1123AB39-E026-4BE2-A10D-2DB9906405A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9020" uniqueCount="4560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9050" uniqueCount="4596">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13555,9 +13555,6 @@
   </si>
   <si>
     <t>Vũ Khúc, Thất Sát đồng cung tại Tật Ách</t>
-  </si>
-  <si>
-    <t>Bệnh ở bộ máy tiêu hóa.</t>
   </si>
   <si>
     <t>yếu thận,  phù chân tay.</t>
@@ -13710,6 +13707,119 @@
   </si>
   <si>
     <t>Tai nạn sông nước, hoặc bị bệnh phong tình</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bệnh ở hạ bộ, mặt thường có vết, lúc ít tuổi có nhiều mụn nhọt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bệnh do tửu sắc gây nên. </t>
+  </si>
+  <si>
+    <t>Cự Môn, Hoá Kỵ đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Dễ đuối nước</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Tật Ách</t>
+  </si>
+  <si>
+    <t>Tật ở đầu hoặc mặt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Da mặt vàng, có bệnh thuộc về khí huyết hay bệnh ngoài da. </t>
+  </si>
+  <si>
+    <t>Thiên Tướng, Vũ Khúc đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Tật ở đầu</t>
+  </si>
+  <si>
+    <t>Thiên Tướng, Thiên Hình đồng cung tại Tật Ách gặp Vũ Khúc</t>
+  </si>
+  <si>
+    <t>Chắc chắn có tật ở đầu</t>
+  </si>
+  <si>
+    <t>Mắc bệnh hàn nhiệt, nhưng không đáng lo ngại.</t>
+  </si>
+  <si>
+    <t>Mặt có bớt, hoặc lúc nhỏ dễ ốm yếu, sức khỏe không tốt</t>
+  </si>
+  <si>
+    <t>Bệnh ở bộ máy tiêu hóa,  thường mắc bệnh trĩ. Nếu 
+không chân tay cũng có thương tích.</t>
+  </si>
+  <si>
+    <t>Thất Sát tọa thủ cung Tật Ách gặp Địa Không, Địa Kiếp, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Mắc tai nạn về súng đạn hay đao thương</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rất dễ  chân tay có thương tật, thường hay mắc tai nạn về đao thương. </t>
+  </si>
+  <si>
+    <t>Thất Sát tọa thủ cung Tật Ách gặp Hoá Kỵ, Đà La</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bệnh tật ở mặt. </t>
+  </si>
+  <si>
+    <t>Thất Sát tọa thủ cung Tật Ách gặp Đà La, Phá Quân, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Dễ mắc tù tội, lao lý</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Tật Ách</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Máu nóng, nên lúc ít tuổi có nhiều mụn nhọt, chóc lở. Lớn lên lại hay mắc tai nạn xe cộ. Nếu không cũng khó tránh được tù tội. </t>
+  </si>
+  <si>
+    <t>Vũ Khúc, Phá Quân đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Mắt kém.</t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Phá Quân đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Chân tay có tỳ vết.</t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Phá Quân, Hỏa Tinh đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Điên cuồng, nếu không, cũng có tật ở mắt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mắc tù tội, bị đánh dập tàn nhẫn. </t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Tật Ách gặp Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Tật Ách gặp các sao Kình Dương, Đà La, Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bị điện giật hay sét đánh rất nguy nan. Nếu không, 
+cũng tai nạn về súng đạn. </t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Tật Ách gặp Thiên Hình, Phục Binh, Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t>Bị sát hại</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Tật Ách gặp Đào Hoa, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>Mắc bệnh phong tình</t>
   </si>
 </sst>
 </file>
@@ -13754,7 +13864,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -14261,10 +14381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A2:B4511"/>
+  <dimension ref="A2:B4526"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4490" workbookViewId="0">
-      <selection activeCell="B4514" sqref="B4514"/>
+    <sheetView tabSelected="1" topLeftCell="A4504" workbookViewId="0">
+      <selection activeCell="E4524" sqref="E4524"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16848,12 +16968,12 @@
         <v>459</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>460</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>460</v>
+        <v>4559</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
@@ -18045,7 +18165,7 @@
         <v>604</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>4539</v>
+        <v>4538</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
@@ -20429,7 +20549,7 @@
         <v>901</v>
       </c>
       <c r="B771" s="1" t="s">
-        <v>901</v>
+        <v>4575</v>
       </c>
     </row>
     <row r="772" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24992,12 +25112,12 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="1342" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1342" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1342" s="1" t="s">
         <v>1452</v>
       </c>
       <c r="B1342" s="1" t="s">
-        <v>1452</v>
+        <v>4571</v>
       </c>
     </row>
     <row r="1343" spans="1:2" x14ac:dyDescent="0.25">
@@ -25517,7 +25637,7 @@
         <v>1517</v>
       </c>
       <c r="B1407" s="1" t="s">
-        <v>1517</v>
+        <v>4591</v>
       </c>
     </row>
     <row r="1408" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -26744,12 +26864,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1561" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1561" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1561" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B1561" s="1" t="s">
-        <v>37</v>
+        <v>4565</v>
       </c>
     </row>
     <row r="1562" spans="1:2" x14ac:dyDescent="0.25">
@@ -34797,7 +34917,7 @@
         <v>2444</v>
       </c>
       <c r="B2567" s="1" t="s">
-        <v>4553</v>
+        <v>4552</v>
       </c>
     </row>
     <row r="2568" spans="1:2" x14ac:dyDescent="0.25">
@@ -34813,7 +34933,7 @@
         <v>2446</v>
       </c>
       <c r="B2569" s="1" t="s">
-        <v>4546</v>
+        <v>4545</v>
       </c>
     </row>
     <row r="2570" spans="1:2" x14ac:dyDescent="0.25">
@@ -34829,7 +34949,7 @@
         <v>2448</v>
       </c>
       <c r="B2571" s="1" t="s">
-        <v>4550</v>
+        <v>4549</v>
       </c>
     </row>
     <row r="2572" spans="1:2" x14ac:dyDescent="0.25">
@@ -34845,7 +34965,7 @@
         <v>2450</v>
       </c>
       <c r="B2573" s="1" t="s">
-        <v>4553</v>
+        <v>4552</v>
       </c>
     </row>
     <row r="2574" spans="1:2" x14ac:dyDescent="0.25">
@@ -34861,7 +34981,7 @@
         <v>2452</v>
       </c>
       <c r="B2575" s="1" t="s">
-        <v>4546</v>
+        <v>4545</v>
       </c>
     </row>
     <row r="2576" spans="1:2" x14ac:dyDescent="0.25">
@@ -34877,7 +34997,7 @@
         <v>2454</v>
       </c>
       <c r="B2577" s="1" t="s">
-        <v>4550</v>
+        <v>4549</v>
       </c>
     </row>
     <row r="2578" spans="1:2" x14ac:dyDescent="0.25">
@@ -35008,12 +35128,12 @@
         <v>2470</v>
       </c>
     </row>
-    <row r="2594" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2594" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2594" s="1" t="s">
         <v>2471</v>
       </c>
       <c r="B2594" s="1" t="s">
-        <v>2471</v>
+        <v>4565</v>
       </c>
     </row>
     <row r="2595" spans="1:2" x14ac:dyDescent="0.25">
@@ -35077,7 +35197,7 @@
         <v>2479</v>
       </c>
       <c r="B2602" s="1" t="s">
-        <v>2479</v>
+        <v>4570</v>
       </c>
     </row>
     <row r="2603" spans="1:2" x14ac:dyDescent="0.25">
@@ -35085,7 +35205,7 @@
         <v>2480</v>
       </c>
       <c r="B2603" s="1" t="s">
-        <v>2480</v>
+        <v>4570</v>
       </c>
     </row>
     <row r="2604" spans="1:2" x14ac:dyDescent="0.25">
@@ -35165,7 +35285,7 @@
         <v>2490</v>
       </c>
       <c r="B2613" s="1" t="s">
-        <v>2490</v>
+        <v>4570</v>
       </c>
     </row>
     <row r="2614" spans="1:2" x14ac:dyDescent="0.25">
@@ -44301,7 +44421,7 @@
         <v>3753</v>
       </c>
       <c r="B3755" s="1" t="s">
-        <v>3753</v>
+        <v>4560</v>
       </c>
     </row>
     <row r="3756" spans="1:2" x14ac:dyDescent="0.25">
@@ -50144,12 +50264,12 @@
         <v>4507</v>
       </c>
     </row>
-    <row r="4486" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4486" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4486" s="1" t="s">
         <v>4508</v>
       </c>
       <c r="B4486" s="1" t="s">
-        <v>4509</v>
+        <v>4572</v>
       </c>
     </row>
     <row r="4487" spans="1:2" x14ac:dyDescent="0.25">
@@ -50157,55 +50277,55 @@
         <v>3741</v>
       </c>
       <c r="B4487" s="1" t="s">
-        <v>4510</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="4488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4488" s="1" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
       <c r="B4488" s="1" t="s">
-        <v>4511</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="4489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4489" s="1" t="s">
+        <v>4511</v>
+      </c>
+      <c r="B4489" s="1" t="s">
         <v>4512</v>
-      </c>
-      <c r="B4489" s="1" t="s">
-        <v>4513</v>
       </c>
     </row>
     <row r="4490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4490" s="1" t="s">
+        <v>4513</v>
+      </c>
+      <c r="B4490" s="1" t="s">
         <v>4514</v>
-      </c>
-      <c r="B4490" s="1" t="s">
-        <v>4515</v>
       </c>
     </row>
     <row r="4491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4491" s="1" t="s">
+        <v>4515</v>
+      </c>
+      <c r="B4491" s="1" t="s">
         <v>4516</v>
-      </c>
-      <c r="B4491" s="1" t="s">
-        <v>4517</v>
       </c>
     </row>
     <row r="4492" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4492" s="1" t="s">
+        <v>4517</v>
+      </c>
+      <c r="B4492" s="1" t="s">
         <v>4518</v>
-      </c>
-      <c r="B4492" s="1" t="s">
-        <v>4519</v>
       </c>
     </row>
     <row r="4493" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4493" s="1" t="s">
+        <v>4519</v>
+      </c>
+      <c r="B4493" s="1" t="s">
         <v>4520</v>
-      </c>
-      <c r="B4493" s="1" t="s">
-        <v>4521</v>
       </c>
     </row>
     <row r="4494" spans="1:2" x14ac:dyDescent="0.25">
@@ -50213,200 +50333,323 @@
         <v>3744</v>
       </c>
       <c r="B4494" s="1" t="s">
-        <v>4522</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="4495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4495" s="1" t="s">
-        <v>4523</v>
+        <v>4522</v>
       </c>
       <c r="B4495" s="1" t="s">
-        <v>4526</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="4496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4496" s="1" t="s">
+        <v>4523</v>
+      </c>
+      <c r="B4496" s="1" t="s">
         <v>4524</v>
-      </c>
-      <c r="B4496" s="1" t="s">
-        <v>4525</v>
       </c>
     </row>
     <row r="4497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4497" s="1" t="s">
+        <v>4526</v>
+      </c>
+      <c r="B4497" s="1" t="s">
         <v>4527</v>
-      </c>
-      <c r="B4497" s="1" t="s">
-        <v>4528</v>
       </c>
     </row>
     <row r="4498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4498" s="1" t="s">
+        <v>4528</v>
+      </c>
+      <c r="B4498" s="1" t="s">
         <v>4529</v>
-      </c>
-      <c r="B4498" s="1" t="s">
-        <v>4530</v>
       </c>
     </row>
     <row r="4499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4499" s="1" t="s">
+        <v>4530</v>
+      </c>
+      <c r="B4499" s="1" t="s">
         <v>4531</v>
-      </c>
-      <c r="B4499" s="1" t="s">
-        <v>4532</v>
       </c>
     </row>
     <row r="4500" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4500" s="1" t="s">
+        <v>4532</v>
+      </c>
+      <c r="B4500" s="1" t="s">
         <v>4533</v>
-      </c>
-      <c r="B4500" s="1" t="s">
-        <v>4534</v>
       </c>
     </row>
     <row r="4501" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4501" s="1" t="s">
+        <v>4534</v>
+      </c>
+      <c r="B4501" s="1" t="s">
         <v>4535</v>
-      </c>
-      <c r="B4501" s="1" t="s">
-        <v>4536</v>
       </c>
     </row>
     <row r="4502" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4502" s="1" t="s">
+        <v>4536</v>
+      </c>
+      <c r="B4502" s="1" t="s">
         <v>4537</v>
-      </c>
-      <c r="B4502" s="1" t="s">
-        <v>4538</v>
       </c>
     </row>
     <row r="4503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4503" s="1" t="s">
+        <v>4539</v>
+      </c>
+      <c r="B4503" s="1" t="s">
         <v>4540</v>
-      </c>
-      <c r="B4503" s="1" t="s">
-        <v>4541</v>
       </c>
     </row>
     <row r="4504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4504" s="1" t="s">
+        <v>4541</v>
+      </c>
+      <c r="B4504" s="1" t="s">
         <v>4542</v>
-      </c>
-      <c r="B4504" s="1" t="s">
-        <v>4543</v>
       </c>
     </row>
     <row r="4505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4505" s="1" t="s">
+        <v>4543</v>
+      </c>
+      <c r="B4505" s="1" t="s">
         <v>4544</v>
-      </c>
-      <c r="B4505" s="1" t="s">
-        <v>4545</v>
       </c>
     </row>
     <row r="4506" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4506" s="1" t="s">
-        <v>4548</v>
+        <v>4547</v>
       </c>
       <c r="B4506" s="1" t="s">
-        <v>4547</v>
+        <v>4546</v>
       </c>
     </row>
     <row r="4507" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4507" s="1" t="s">
-        <v>4549</v>
+        <v>4548</v>
       </c>
       <c r="B4507" s="1" t="s">
-        <v>4547</v>
+        <v>4546</v>
       </c>
     </row>
     <row r="4508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4508" s="1" t="s">
+        <v>4550</v>
+      </c>
+      <c r="B4508" s="1" t="s">
         <v>4551</v>
-      </c>
-      <c r="B4508" s="1" t="s">
-        <v>4552</v>
       </c>
     </row>
     <row r="4509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4509" s="1" t="s">
+        <v>4553</v>
+      </c>
+      <c r="B4509" s="1" t="s">
         <v>4554</v>
-      </c>
-      <c r="B4509" s="1" t="s">
-        <v>4555</v>
       </c>
     </row>
     <row r="4510" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4510" s="1" t="s">
+        <v>4555</v>
+      </c>
+      <c r="B4510" s="1" t="s">
         <v>4556</v>
-      </c>
-      <c r="B4510" s="1" t="s">
-        <v>4557</v>
       </c>
     </row>
     <row r="4511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4511" s="1" t="s">
+        <v>4557</v>
+      </c>
+      <c r="B4511" s="1" t="s">
         <v>4558</v>
       </c>
-      <c r="B4511" s="1" t="s">
-        <v>4559</v>
+    </row>
+    <row r="4512" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4512" s="1" t="s">
+        <v>4561</v>
+      </c>
+      <c r="B4512" s="1" t="s">
+        <v>4562</v>
+      </c>
+    </row>
+    <row r="4513" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4513" s="1" t="s">
+        <v>4563</v>
+      </c>
+      <c r="B4513" s="1" t="s">
+        <v>4564</v>
+      </c>
+    </row>
+    <row r="4514" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4514" s="1" t="s">
+        <v>4566</v>
+      </c>
+      <c r="B4514" s="1" t="s">
+        <v>4567</v>
+      </c>
+    </row>
+    <row r="4515" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4515" s="1" t="s">
+        <v>4568</v>
+      </c>
+      <c r="B4515" s="1" t="s">
+        <v>4569</v>
+      </c>
+    </row>
+    <row r="4516" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4516" s="1" t="s">
+        <v>4573</v>
+      </c>
+      <c r="B4516" s="1" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="4517" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4517" s="1" t="s">
+        <v>4576</v>
+      </c>
+      <c r="B4517" s="1" t="s">
+        <v>4577</v>
+      </c>
+    </row>
+    <row r="4518" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4518" s="1" t="s">
+        <v>4578</v>
+      </c>
+      <c r="B4518" s="1" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="4519" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4519" s="1" t="s">
+        <v>4580</v>
+      </c>
+      <c r="B4519" s="1" t="s">
+        <v>4581</v>
+      </c>
+    </row>
+    <row r="4520" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4520" s="1" t="s">
+        <v>4582</v>
+      </c>
+      <c r="B4520" s="1" t="s">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="4521" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4521" s="1" t="s">
+        <v>4584</v>
+      </c>
+      <c r="B4521" s="1" t="s">
+        <v>4585</v>
+      </c>
+    </row>
+    <row r="4522" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4522" s="1" t="s">
+        <v>4586</v>
+      </c>
+      <c r="B4522" s="1" t="s">
+        <v>4562</v>
+      </c>
+    </row>
+    <row r="4523" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4523" s="1" t="s">
+        <v>4590</v>
+      </c>
+      <c r="B4523" s="1" t="s">
+        <v>4587</v>
+      </c>
+    </row>
+    <row r="4524" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4524" s="1" t="s">
+        <v>4589</v>
+      </c>
+      <c r="B4524" s="1" t="s">
+        <v>4588</v>
+      </c>
+    </row>
+    <row r="4525" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4525" s="1" t="s">
+        <v>4592</v>
+      </c>
+      <c r="B4525" s="1" t="s">
+        <v>4593</v>
+      </c>
+    </row>
+    <row r="4526" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4526" s="1" t="s">
+        <v>4594</v>
+      </c>
+      <c r="B4526" s="1" t="s">
+        <v>4595</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}"/>
   <dataConsolidate/>
   <conditionalFormatting sqref="A25">
-    <cfRule type="duplicateValues" dxfId="22" priority="93"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="94"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="94"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="95"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86:A143">
-    <cfRule type="duplicateValues" dxfId="20" priority="63"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145">
-    <cfRule type="duplicateValues" dxfId="18" priority="67"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A146:A209">
-    <cfRule type="duplicateValues" dxfId="16" priority="62"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1810:A3339">
-    <cfRule type="duplicateValues" dxfId="15" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3853:A3914">
-    <cfRule type="duplicateValues" dxfId="14" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6758:A1048576 A210:A1632 A2:A24 A26:A85 A144 A1805:A1809 A3442:A3852 A3915:A4214">
-    <cfRule type="duplicateValues" dxfId="13" priority="102"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="104"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="105"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86:B143">
-    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B146:B209">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1810:B3339">
     <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1810:B3339">
+  <conditionalFormatting sqref="B3853:B3914">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3853:B3914">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="B6758:B1048576 B210:B1632 B2:B24 B26:B85 B144 B1805:B1809 B3915:B4214 B3442:B3852">
+    <cfRule type="duplicateValues" dxfId="2" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6758:B1048576 B210:B1632 B2:B24 B26:B85 B144 B1805:B1809 B3915:B4214 B3442:B3852">
-    <cfRule type="duplicateValues" dxfId="1" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
+  <conditionalFormatting sqref="B1561">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Giải thích Kình Đà
</commit_message>
<xml_diff>
--- a/LuanTatAch.xlsx
+++ b/LuanTatAch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App_Tuvi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1123AB39-E026-4BE2-A10D-2DB9906405A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047E9991-0CE0-4737-810E-3ACDCB181D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9050" uniqueCount="4596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9072" uniqueCount="4616">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13820,6 +13820,66 @@
   </si>
   <si>
     <t>Mắc bệnh phong tình</t>
+  </si>
+  <si>
+    <t>Kình Dương toạ thủ cung Tật Ách ở Ngọ gặp Thất Sát, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Mắc tù tội hay tai nạn đao thương</t>
+  </si>
+  <si>
+    <t>Kình Dương, Hóa Kỵ đồng cung Tật Ách ở Tỵ</t>
+  </si>
+  <si>
+    <t>Mắt rất kém, hoặc mù lòa</t>
+  </si>
+  <si>
+    <t>Kình Dương, Hóa Kỵ đồng cung Tật Ách ở Hợi</t>
+  </si>
+  <si>
+    <t>Kình Dương toạ thủ cung Tật Ách gặp Hỏa Tinh, Linh Tinh, Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t>Tự sát hoặc bị sát hại</t>
+  </si>
+  <si>
+    <t>Kình Dương, Bạch Hổ đồng cung tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Sẽ bị chó dại cắn</t>
+  </si>
+  <si>
+    <t>Kình Dương toạ thủ cung Tật Ách gặp Hoa Cái, Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bị phát ban hay lên đậu sởi rất đáng lo ngại. </t>
+  </si>
+  <si>
+    <t>Kình Hình</t>
+  </si>
+  <si>
+    <t>Kình Hình hội chiếu tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Dễ bị tai nạn, hỏng xe cộ, tai nạn xe cộ, máy móc</t>
+  </si>
+  <si>
+    <t>Kình Hình Không Kiếp</t>
+  </si>
+  <si>
+    <t>Kình Hình Không Kiếp hội chiếu tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Bị sát hại, hoặc bị đánh đập rất tàn bạo</t>
+  </si>
+  <si>
+    <t>Kình Dương, Thái Tuế đồng cung Tật Ách</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mắc kiện cáo, tù tội. </t>
+  </si>
+  <si>
+    <t>Mắc bệnh ở tai, thường có bệnh trĩ, nếu không, cũng có tỳ vết ở chân.</t>
   </si>
 </sst>
 </file>
@@ -14381,10 +14441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A2:B4526"/>
+  <dimension ref="A2:B4537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4504" workbookViewId="0">
-      <selection activeCell="E4524" sqref="E4524"/>
+    <sheetView tabSelected="1" topLeftCell="A4526" workbookViewId="0">
+      <selection activeCell="F4538" sqref="F4538"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30832,12 +30892,12 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="2057" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2057" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2057" s="1" t="s">
         <v>2055</v>
       </c>
       <c r="B2057" s="1" t="s">
-        <v>2055</v>
+        <v>4615</v>
       </c>
     </row>
     <row r="2058" spans="1:2" x14ac:dyDescent="0.25">
@@ -50590,6 +50650,94 @@
       </c>
       <c r="B4526" s="1" t="s">
         <v>4595</v>
+      </c>
+    </row>
+    <row r="4527" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4527" s="1" t="s">
+        <v>4596</v>
+      </c>
+      <c r="B4527" s="1" t="s">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="4528" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4528" s="1" t="s">
+        <v>4598</v>
+      </c>
+      <c r="B4528" s="1" t="s">
+        <v>4599</v>
+      </c>
+    </row>
+    <row r="4529" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4529" s="1" t="s">
+        <v>4600</v>
+      </c>
+      <c r="B4529" s="1" t="s">
+        <v>4599</v>
+      </c>
+    </row>
+    <row r="4530" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4530" s="1" t="s">
+        <v>4601</v>
+      </c>
+      <c r="B4530" s="1" t="s">
+        <v>4602</v>
+      </c>
+    </row>
+    <row r="4531" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4531" s="1" t="s">
+        <v>4603</v>
+      </c>
+      <c r="B4531" s="1" t="s">
+        <v>4604</v>
+      </c>
+    </row>
+    <row r="4532" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4532" s="1" t="s">
+        <v>4605</v>
+      </c>
+      <c r="B4532" s="1" t="s">
+        <v>4606</v>
+      </c>
+    </row>
+    <row r="4533" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4533" s="1" t="s">
+        <v>4607</v>
+      </c>
+      <c r="B4533" s="1" t="s">
+        <v>4607</v>
+      </c>
+    </row>
+    <row r="4534" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4534" s="1" t="s">
+        <v>4608</v>
+      </c>
+      <c r="B4534" s="1" t="s">
+        <v>4609</v>
+      </c>
+    </row>
+    <row r="4535" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4535" s="1" t="s">
+        <v>4610</v>
+      </c>
+      <c r="B4535" s="1" t="s">
+        <v>4610</v>
+      </c>
+    </row>
+    <row r="4536" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4536" s="1" t="s">
+        <v>4611</v>
+      </c>
+      <c r="B4536" s="1" t="s">
+        <v>4612</v>
+      </c>
+    </row>
+    <row r="4537" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4537" s="1" t="s">
+        <v>4613</v>
+      </c>
+      <c r="B4537" s="1" t="s">
+        <v>4614</v>
       </c>
     </row>
   </sheetData>
@@ -50616,7 +50764,7 @@
   <conditionalFormatting sqref="A3853:A3914">
     <cfRule type="duplicateValues" dxfId="15" priority="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6758:A1048576 A210:A1632 A2:A24 A26:A85 A144 A1805:A1809 A3442:A3852 A3915:A4214">
+  <conditionalFormatting sqref="A6757:A1048576 A210:A1632 A2:A24 A26:A85 A144 A1805:A1809 A3442:A3852 A3915:A4214">
     <cfRule type="duplicateValues" dxfId="14" priority="103"/>
     <cfRule type="duplicateValues" dxfId="13" priority="105"/>
   </conditionalFormatting>
@@ -50644,7 +50792,7 @@
   <conditionalFormatting sqref="B3853:B3914">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6758:B1048576 B210:B1632 B2:B24 B26:B85 B144 B1805:B1809 B3915:B4214 B3442:B3852">
+  <conditionalFormatting sqref="B6757:B1048576 B210:B1632 B2:B24 B26:B85 B144 B1805:B1809 B3915:B4214 B3442:B3852">
     <cfRule type="duplicateValues" dxfId="2" priority="12"/>
     <cfRule type="duplicateValues" dxfId="1" priority="13"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
nao sua lai ta phu them cac cach cuc xoa bo cach cuc khong pho bien
</commit_message>
<xml_diff>
--- a/LuanTatAch.xlsx
+++ b/LuanTatAch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App_Tuvi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2A922D-E538-4DF0-BC2F-A10915AC940B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE5FFF9-55A5-4F0F-9CD8-DD902D277641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="3375" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -14981,8 +14981,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:D4606"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2242" workbookViewId="0">
-      <selection activeCell="C2374" sqref="C2374"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C1612" sqref="C1612"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>